<commit_message>
RMA information Save/ Load 가능. (include contents, Bill, ship information) History(Related RMA information) Panel query and click
</commit_message>
<xml_diff>
--- a/src/Database Structure.xlsx
+++ b/src/Database Structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="72" windowWidth="23256" windowHeight="13116" activeTab="5"/>
+    <workbookView xWindow="195" yWindow="75" windowWidth="23250" windowHeight="13110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="7" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="RMA_ITEM table" sheetId="6" r:id="rId5"/>
     <sheet name="RMA Table" sheetId="1" r:id="rId6"/>
     <sheet name="Case Table" sheetId="3" r:id="rId7"/>
+    <sheet name="Goal" sheetId="8" r:id="rId8"/>
+    <sheet name="정규화" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,10 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">Primary Key </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Site</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -196,14 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>    `companySiteName` CHAR(100) NOT NULL,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alter table company add foreign key (companySiteName) references site(siteName);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>companyName</t>
   </si>
   <si>
@@ -220,9 +210,6 @@
   </si>
   <si>
     <t>companyEmail</t>
-  </si>
-  <si>
-    <t>companySiteName</t>
   </si>
   <si>
     <t>    `companyCity` CHAR(100) NOT NULL, </t>
@@ -444,6 +431,314 @@
     <t>ALTER TABLE rma_table DROP rmaItem;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">단기 목표 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TextArea 에서 Tab키를 포커스 이동용으로 만들기.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">종료될때 마지막(?) 혹은 사용되지않은 preserved 개체들 삭제하기. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>History Panel쪽의 리스트 레이아웃 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이아웃 크기조절 가능하게 변경하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C#으로 포팅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">장기 목표 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">각 항목들 작성할때 mysql에서 이전에 저장된 데이터 불러와서 보여주기. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">완료 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">RMA preserve 단계에서 어떻게 저장할것인지 고민. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버가 실행될때 테이블이 존재하는지 확인하고 생성하는 쿼리 필요할듯. (재설치)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+테이블 생성할때 RMA preserve용 값을 하나 insert한다(company, site)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">완료. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">해결방법. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">TextArea에 KeyAdapter객체를 추가. 
+Press된 키가 tab일때 동작을 변경. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장하고 지워버림.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Global variable, local variable 코드 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">클라이언트에서 서버에 접속할때, 연결을 반복하는것과 무한루프로 입력을 기다리는것 
+중 어느것이 부하가 적을것인가 확인해보기 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Jtable 편의성 고려하기. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">문제점 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>garbage 값을 insert 한다음 remove하는 방식으로 
+특정 RMA number를 유지시키되, 저장은 하지않게함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저장하지않고 지우고 넘어가는 경우에도, auto_increment는 다음 번호를 가르키기때문에, 사용되지않는 RMA number가 다수 발생.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">select siteName from site where siteName LIKE 'si%';
+DocumentListener 사용. Insert Update와 remove Update를 이용해서 comboBox에 적히는 keyword를 기준으로 mysql 에 저장되어있는 이름을 검색후 리턴. Drop down list에 추가한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">기본적으로 combobox 리스트에 항목이 추가되면, 그 첫번째 아이템을 selectedItem으로 간주하게 되는데.. 그럴경우 작성하던 검색어가 사라져버림으로 작성하던 text를 유지해야할 필요가있다. 해당 사항으로 고생이 많았으나, comboBoxmodel로 문제해결. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompanyName or SiteName이 검색되었을때, 해당 조건에 맞는 정보를 찾아서 Form에 뿌려주는 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이거때매 고생을 많이함. 병크가 겹쳣던듯.. 규명 불가능. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">company name </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company zipcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>company email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purelink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ramsey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ramsey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMA Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OrderNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contents</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BillTo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ship to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>    `companyName` CHAR(100) NOT NULL, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alter table site add foreign key (companyName) references company(companyName);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA2010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA3010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA4010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>City</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회사코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site 코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">company 1 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site code 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">site code 2 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">site code 1 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>    `siteCode` int(11) Auto_increment, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>    PRIMARY KEY(`siteCode`) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SiteCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -501,7 +796,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -518,6 +813,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -820,65 +1133,65 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="4" max="4" width="20.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="D10" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="F12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="E13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="D14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="D15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="E16" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="6:6">
       <c r="F17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="6:6">
       <c r="F18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -889,109 +1202,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1003,92 +1304,101 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:11">
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11">
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
+    <row r="9" spans="1:11">
+      <c r="B9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
+    <row r="10" spans="1:11">
+      <c r="B10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>36</v>
+    <row r="11" spans="1:11">
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="H10" s="1" t="s">
-        <v>37</v>
+    <row r="12" spans="1:11">
+      <c r="I12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="H11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="H12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>45</v>
+    <row r="16" spans="1:11">
+      <c r="B16" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1102,61 +1412,61 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A7:A11"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1173,100 +1483,100 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" customWidth="1"/>
-    <col min="4" max="4" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16384">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:16384">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:16384">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:16384">
       <c r="A11" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:16384">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:16384">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -17654,37 +17964,37 @@
     </row>
     <row r="14" spans="1:16384">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:16384">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:16384">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -17695,192 +18005,188 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="B8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="B14" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="16.899999999999999" customHeight="1">
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="B7" s="1" t="s">
-        <v>61</v>
+    <row r="31" spans="2:7">
+      <c r="B31" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="B9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="B13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="B14" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="16.95" customHeight="1">
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8">
-      <c r="B28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:7">
       <c r="B32" t="s">
-        <v>106</v>
-      </c>
-      <c r="H32" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="G32" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -17898,21 +18204,21 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -17920,11 +18226,796 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:H32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="25.15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="13.625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="4.125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="72" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="9"/>
+    <col min="5" max="5" width="8.75" style="6"/>
+    <col min="6" max="6" width="47.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.25" style="6" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="8.75" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" ht="25.15" customHeight="1">
+      <c r="C3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="33">
+      <c r="A5" s="7">
+        <v>42816</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="77.25" customHeight="1">
+      <c r="B6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="99">
+      <c r="B7" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.15" customHeight="1">
+      <c r="A9" s="7">
+        <v>42817</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="25.15" customHeight="1">
+      <c r="B10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="33">
+      <c r="A12" s="7">
+        <v>42818</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.15" customHeight="1">
+      <c r="B13" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25.15" customHeight="1">
+      <c r="C23" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25.15" customHeight="1">
+      <c r="A24" s="7">
+        <v>42816</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="25.15" customHeight="1">
+      <c r="B25" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25.15" customHeight="1">
+      <c r="B26" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="25.15" customHeight="1">
+      <c r="B27" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="25.15" customHeight="1">
+      <c r="B28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25.15" customHeight="1">
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" ht="25.15" customHeight="1">
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" ht="49.5">
+      <c r="A31" s="7">
+        <v>42817</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="25.15" customHeight="1">
+      <c r="B32" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B1:B12 B14:B1048576" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:S30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="16384" width="18.25" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" ht="29.25" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K3" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K4" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K5" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L14" s="11">
+        <v>7446</v>
+      </c>
+      <c r="M14" s="11">
+        <v>3232</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>1</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L15" s="11">
+        <v>7446</v>
+      </c>
+      <c r="M15" s="11">
+        <v>3232</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O15" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>2</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11">
+        <v>2</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>3</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C17" s="11">
+        <v>3</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="J29" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="J30" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sign In/Up feature complete.
</commit_message>
<xml_diff>
--- a/src/Database Structure.xlsx
+++ b/src/Database Structure.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="22200" windowHeight="6480" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="22200" windowHeight="6480" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DATABASE" sheetId="7" r:id="rId1"/>
-    <sheet name="Company Table" sheetId="2" r:id="rId2"/>
-    <sheet name="Site Table" sheetId="4" r:id="rId3"/>
-    <sheet name="Item Table" sheetId="5" r:id="rId4"/>
-    <sheet name="RMA_ITEM table" sheetId="6" r:id="rId5"/>
-    <sheet name="RMA Table" sheetId="1" r:id="rId6"/>
-    <sheet name="Case Table" sheetId="3" r:id="rId7"/>
-    <sheet name="Goal" sheetId="8" r:id="rId8"/>
-    <sheet name="정규화" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId2"/>
+    <sheet name="Company Table" sheetId="2" r:id="rId3"/>
+    <sheet name="Site Table" sheetId="4" r:id="rId4"/>
+    <sheet name="Item Table" sheetId="5" r:id="rId5"/>
+    <sheet name="RMA_ITEM table" sheetId="6" r:id="rId6"/>
+    <sheet name="RMA Table" sheetId="1" r:id="rId7"/>
+    <sheet name="Case Table" sheetId="3" r:id="rId8"/>
+    <sheet name="Goal" sheetId="8" r:id="rId9"/>
+    <sheet name="정규화" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="640">
   <si>
     <t>RMA number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2098,35 +2099,267 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RMA 정보 저장할때 날짜 저장될수 있도록.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자형식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA 추가한 형식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">같은 아이템이 두번 나갈수도있으니까, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">시리얼 + RMA넘버가 primary key </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <r>
+      <t>CREATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> user_ID_Table (</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  id CHAR(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF666666"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF880000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PRIMARY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (id)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  passWord VAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFB00040"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CHAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(255) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NOT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF880000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>NULL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000A19"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 첨부 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RMA 정보 저장할때 날짜 저장될수 있도록.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>숫자형식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DA 추가한 형식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Receive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">같은 아이템이 두번 나갈수도있으니까, </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">시리얼 + RMA넘버가 primary key </t>
+    <t xml:space="preserve">원하는 형태로 프린트 할수 있는 기능. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2134,7 +2367,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2175,6 +2408,37 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000A19"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFB00040"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF666666"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF880000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2201,7 +2465,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2240,6 +2504,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2610,13 +2880,642 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A2:S30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="16384" width="18.25" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" ht="29.25" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K3" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K4" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K5" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="11">
+        <v>7446</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3232</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14" s="11">
+        <v>7446</v>
+      </c>
+      <c r="M14" s="11">
+        <v>3232</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="O14" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>1</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" s="11">
+        <v>7446</v>
+      </c>
+      <c r="M15" s="11">
+        <v>3232</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="O15" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>2</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11">
+        <v>2</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>3</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C17" s="11">
+        <v>3</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C19" s="11">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="J29" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M29" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="J30" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="3:4">
+      <c r="C1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4">
+      <c r="C4" s="13" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="14" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="14" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" s="14" t="s">
+        <v>631</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2713,7 +3612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K16"/>
@@ -2819,7 +3718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D417"/>
@@ -7707,12 +8606,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:XFD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -7742,7 +8641,7 @@
         <v>185</v>
       </c>
       <c r="F1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="2" spans="1:16384">
@@ -7753,7 +8652,7 @@
         <v>180</v>
       </c>
       <c r="F2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:16384">
@@ -7782,12 +8681,12 @@
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="10" spans="1:16384">
@@ -24243,7 +25142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K33"/>
@@ -24325,10 +25224,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>623</v>
+      </c>
+      <c r="B4" t="s">
         <v>624</v>
-      </c>
-      <c r="B4" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -24445,7 +25344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C2"/>
@@ -24485,14 +25384,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="A32:XFD32"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
@@ -24766,82 +25665,101 @@
         <v>42867</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" customHeight="1">
-      <c r="C34" s="6" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1">
+      <c r="A32" s="7">
+        <v>42892</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" customHeight="1">
+      <c r="B33" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" customHeight="1">
+      <c r="C35" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" customHeight="1">
-      <c r="A35" s="7">
+    <row r="36" spans="1:3" ht="30" customHeight="1">
+      <c r="A36" s="7">
         <v>42816</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" customHeight="1">
-      <c r="B36" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" customHeight="1">
       <c r="B37" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" customHeight="1">
       <c r="B38" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" customHeight="1">
       <c r="B39" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" customHeight="1">
+      <c r="B40" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" customHeight="1">
-      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" ht="30" customHeight="1">
       <c r="C41" s="10"/>
     </row>
     <row r="42" spans="1:3" ht="30" customHeight="1">
-      <c r="A42" s="7">
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="1:3" ht="30" customHeight="1">
+      <c r="A43" s="7">
         <v>42817</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" customHeight="1">
-      <c r="B43" s="8" t="s">
+    <row r="44" spans="1:3" ht="30" customHeight="1">
+      <c r="B44" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -24850,586 +25768,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:B10 B12 B17 B15 B33:B1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B10 B12 B17 B15 B34:B1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A2:S30"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18.25" defaultRowHeight="16.5"/>
-  <cols>
-    <col min="1" max="16384" width="18.25" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:19" ht="29.25" customHeight="1">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J3" s="11">
-        <v>7446</v>
-      </c>
-      <c r="K3" s="11">
-        <v>3232</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="11">
-        <v>7446</v>
-      </c>
-      <c r="K4" s="11">
-        <v>3232</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="11">
-        <v>7446</v>
-      </c>
-      <c r="K5" s="11">
-        <v>3232</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C6" s="11">
-        <v>3</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C7" s="11">
-        <v>3</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C8" s="11">
-        <v>2</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J8" s="11">
-        <v>7446</v>
-      </c>
-      <c r="K8" s="11">
-        <v>3232</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C9" s="11">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" s="11">
-        <v>7446</v>
-      </c>
-      <c r="K9" s="11">
-        <v>3232</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q13" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="R13" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="S13" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="11">
-        <v>1</v>
-      </c>
-      <c r="I14" s="11">
-        <v>1</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L14" s="11">
-        <v>7446</v>
-      </c>
-      <c r="M14" s="11">
-        <v>3232</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="O14" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>1</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="S14" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="I15" s="11">
-        <v>1</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L15" s="11">
-        <v>7446</v>
-      </c>
-      <c r="M15" s="11">
-        <v>3232</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="O15" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>2</v>
-      </c>
-      <c r="R15" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="S15" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="G16" s="11">
-        <v>1</v>
-      </c>
-      <c r="I16" s="11">
-        <v>2</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="L16" s="11">
-        <v>0</v>
-      </c>
-      <c r="O16" s="11">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>3</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B17" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C17" s="11">
-        <v>3</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C18" s="11">
-        <v>3</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C19" s="11">
-        <v>2</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B20" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C20" s="11">
-        <v>2</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G20" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="J29" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="M29" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="J30" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>